<commit_message>
reading settings from file
</commit_message>
<xml_diff>
--- a/src/test/resources/tests_excels/countryTestCases.xlsx
+++ b/src/test/resources/tests_excels/countryTestCases.xlsx
@@ -9,17 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test cases" sheetId="1" r:id="rId1"/>
+    <sheet name="settings" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
   <si>
     <t>statusCode</t>
   </si>
@@ -27,6 +34,12 @@
     <t>errorMessage</t>
   </si>
   <si>
+    <t>daulet2030@gmail.com</t>
+  </si>
+  <si>
+    <t>TechnoStudy123@</t>
+  </si>
+  <si>
     <t>NULL</t>
   </si>
   <si>
@@ -49,13 +62,25 @@
   </si>
   <si>
     <t>error.validation</t>
+  </si>
+  <si>
+    <t>baseURI</t>
+  </si>
+  <si>
+    <t>https://test.campus.techno.study</t>
+  </si>
+  <si>
+    <t>apiPath</t>
+  </si>
+  <si>
+    <t>/school-service/api/countries/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +215,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15.8"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +400,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -532,9 +575,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -858,11 +907,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -870,77 +919,133 @@
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4">
+        <v>201</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>400</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4">
+        <v>400</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4">
+        <v>400</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4">
         <v>201</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="C3">
-        <v>400</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>400</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>400</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>201</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>